<commit_message>
handled numeric to String Comparison
</commit_message>
<xml_diff>
--- a/vtigerCRM/src/test/resources/TestData/TestScriptData.xlsx
+++ b/vtigerCRM/src/test/resources/TestData/TestScriptData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisha\git\repository6\vtigerCRM\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01351BBB-B501-418F-8790-481C01897367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D5943A-EE20-415E-A741-6B466D1E81A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{CFB00352-CA09-4FD1-8543-BA29FA27DC52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CFB00352-CA09-4FD1-8543-BA29FA27DC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -601,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -670,18 +670,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1064,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFCF65F-B9C5-4398-BF22-01F216CDE7F6}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="62" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="62" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,10 +1118,10 @@
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -1129,8 +1132,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="15" t="s">
         <v>6</v>
       </c>
@@ -1139,8 +1142,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="16" t="s">
         <v>19</v>
       </c>
@@ -1149,8 +1152,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="39"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="16" t="s">
         <v>20</v>
       </c>
@@ -1159,8 +1162,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
@@ -1169,8 +1172,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
@@ -1179,8 +1182,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
-      <c r="B11" s="39"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="16" t="s">
         <v>23</v>
       </c>
@@ -1189,12 +1192,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="30" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1222,10 +1225,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="35" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -1236,52 +1239,52 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="32">
         <v>9999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="32">
         <v>8888888888</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="32">
         <v>7777777777</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="32">
         <v>6666666666</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="33">
         <v>5555555555</v>
       </c>
     </row>
@@ -1289,7 +1292,7 @@
       <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D24" s="29"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
@@ -1306,10 +1309,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="35" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -1320,8 +1323,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="15" t="s">
         <v>45</v>
       </c>
@@ -1330,8 +1333,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="16" t="s">
         <v>46</v>
       </c>
@@ -1360,10 +1363,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="35" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="15" t="s">
@@ -1374,8 +1377,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="15" t="s">
         <v>6</v>
       </c>
@@ -1384,8 +1387,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="15" t="s">
         <v>48</v>
       </c>
@@ -1414,10 +1417,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="38" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="15" t="s">
@@ -1428,12 +1431,12 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
-      <c r="B39" s="38"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="39"/>
       <c r="C39" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="29">
         <v>32168</v>
       </c>
     </row>
@@ -1447,7 +1450,7 @@
       <c r="D42" s="24"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D43" s="29"/>
+      <c r="D43" s="28"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
@@ -1464,10 +1467,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="35" t="s">
         <v>50</v>
       </c>
       <c r="C45" s="15" t="s">
@@ -1478,8 +1481,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="15" t="s">
         <v>18</v>
       </c>
@@ -1488,8 +1491,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
       <c r="C47" s="15" t="s">
         <v>6</v>
       </c>
@@ -1498,8 +1501,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="35"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
       <c r="C48" s="15" t="s">
         <v>45</v>
       </c>
@@ -1508,8 +1511,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="35"/>
-      <c r="B49" s="35"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="15" t="s">
         <v>48</v>
       </c>
@@ -1518,8 +1521,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="35"/>
-      <c r="B50" s="35"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
       <c r="C50" s="16" t="s">
         <v>19</v>
       </c>
@@ -1528,8 +1531,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="35"/>
-      <c r="B51" s="35"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
       <c r="C51" s="16" t="s">
         <v>20</v>
       </c>
@@ -1538,8 +1541,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="35"/>
-      <c r="B52" s="35"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="36"/>
       <c r="C52" s="16" t="s">
         <v>21</v>
       </c>
@@ -1548,8 +1551,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="35"/>
-      <c r="B53" s="35"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="16" t="s">
         <v>22</v>
       </c>
@@ -1558,58 +1561,58 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="35"/>
-      <c r="B54" s="35"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D54" s="34">
         <v>99999999999</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="35"/>
-      <c r="B55" s="35"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D55" s="15">
+      <c r="D55" s="34">
         <v>88888888888</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="35"/>
-      <c r="B56" s="35"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="15">
+      <c r="D56" s="34">
         <v>77777777777</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="35"/>
-      <c r="B57" s="35"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="34">
         <v>66666666666</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="35"/>
-      <c r="B58" s="35"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="36"/>
       <c r="C58" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="15">
+      <c r="D58" s="34">
         <v>55555555555</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="35"/>
-      <c r="B59" s="35"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="16" t="s">
         <v>23</v>
       </c>
@@ -1618,8 +1621,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="35"/>
-      <c r="B60" s="35"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
       <c r="C60" s="16" t="s">
         <v>43</v>
       </c>
@@ -1628,8 +1631,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="35"/>
-      <c r="B61" s="35"/>
+      <c r="A61" s="36"/>
+      <c r="B61" s="36"/>
       <c r="C61" s="16" t="s">
         <v>46</v>
       </c>
@@ -1638,8 +1641,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
       <c r="C62" s="16" t="s">
         <v>24</v>
       </c>
@@ -1731,10 +1734,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
@@ -1745,8 +1748,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" t="s">
         <v>67</v>
       </c>
@@ -1755,8 +1758,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
       <c r="C8" t="s">
         <v>69</v>
       </c>
@@ -1765,9 +1768,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="41"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33" t="s">
+      <c r="A9" s="42"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
         <v>71</v>
       </c>
       <c r="D9" t="s">
@@ -1775,10 +1778,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
     </row>
     <row r="11" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
made changes in Organization modules
</commit_message>
<xml_diff>
--- a/vtigerCRM/src/test/resources/TestData/TestScriptData.xlsx
+++ b/vtigerCRM/src/test/resources/TestData/TestScriptData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisha\git\repository6\vtigerCRM\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D5943A-EE20-415E-A741-6B466D1E81A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2270CB93-9155-4570-9E39-B48D4B8A5184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CFB00352-CA09-4FD1-8543-BA29FA27DC52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CFB00352-CA09-4FD1-8543-BA29FA27DC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
   <si>
     <t>ExpectedTitle</t>
   </si>
@@ -258,6 +258,54 @@
   </si>
   <si>
     <t>Potter</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Competiitor</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Integrator</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>Prospect</t>
+  </si>
+  <si>
+    <t>Reseller</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Market Failed</t>
+  </si>
+  <si>
+    <t>Project Cancelled</t>
+  </si>
+  <si>
+    <t>Shutdown</t>
   </si>
 </sst>
 </file>
@@ -697,10 +745,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1067,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFCF65F-B9C5-4398-BF22-01F216CDE7F6}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="62" workbookViewId="0">
+    <sheetView zoomScale="62" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -1133,7 +1181,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="36"/>
-      <c r="B6" s="40"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="15" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +1191,7 @@
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
-      <c r="B7" s="40"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="16" t="s">
         <v>19</v>
       </c>
@@ -1153,7 +1201,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="36"/>
-      <c r="B8" s="40"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="16" t="s">
         <v>20</v>
       </c>
@@ -1163,7 +1211,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="36"/>
-      <c r="B9" s="40"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
@@ -1173,7 +1221,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
-      <c r="B10" s="40"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
@@ -1183,7 +1231,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="36"/>
-      <c r="B11" s="40"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="16" t="s">
         <v>23</v>
       </c>
@@ -1193,7 +1241,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="37"/>
-      <c r="B12" s="39"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1432,7 +1480,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="37"/>
-      <c r="B39" s="39"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="15" t="s">
         <v>43</v>
       </c>
@@ -1652,18 +1700,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A45:A62"/>
+    <mergeCell ref="B45:B62"/>
     <mergeCell ref="A5:A12"/>
     <mergeCell ref="B5:B12"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A45:A62"/>
-    <mergeCell ref="B45:B62"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{692FCA9A-91E4-4CA6-BA24-3480D75BBC0D}"/>
@@ -1676,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBDE8C7-8843-4568-A5EB-0912EF09EE33}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,9 +1736,11 @@
     <col min="2" max="2" width="60.77734375" customWidth="1"/>
     <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1704,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1718,8 +1768,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1733,7 +1783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
         <v>15</v>
       </c>
@@ -1747,7 +1797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="36"/>
       <c r="B7" s="36"/>
       <c r="C7" t="s">
@@ -1756,8 +1806,17 @@
       <c r="D7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="36"/>
       <c r="B8" s="36"/>
       <c r="C8" t="s">
@@ -1766,8 +1825,35 @@
       <c r="D8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="42"/>
       <c r="B9" s="31"/>
       <c r="C9" s="31" t="s">
@@ -1776,11 +1862,23 @@
       <c r="D9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36"/>
     </row>
-    <row r="11" spans="1:4" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="43"/>
     </row>
   </sheetData>

</xml_diff>